<commit_message>
Update Evaluation Result Updated.xlsx
</commit_message>
<xml_diff>
--- a/Document/Final_Documents_Capstone/Evaluation Result Updated.xlsx
+++ b/Document/Final_Documents_Capstone/Evaluation Result Updated.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jhel\Desktop\CapstoneChap4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\VirtualShrine\Document\Final_Documents_Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -962,6 +962,18 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="10" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="40" xfId="11"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="41" xfId="12" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1040,6 +1052,7 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1057,19 +1070,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="10" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="40" xfId="11"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="41" xfId="12" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1377,8 +1377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="W49" sqref="W49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1391,97 +1391,97 @@
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="108" t="s">
+      <c r="C2" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="110"/>
-      <c r="G2" s="114" t="s">
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="115"/>
-      <c r="I2" s="115"/>
-      <c r="J2" s="115"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="120" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="121"/>
-      <c r="N2" s="121"/>
-      <c r="O2" s="122"/>
-      <c r="P2" s="126" t="s">
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="124"/>
+      <c r="L2" s="128" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="129"/>
+      <c r="N2" s="129"/>
+      <c r="O2" s="130"/>
+      <c r="P2" s="135" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="127"/>
-      <c r="R2" s="127"/>
-      <c r="S2" s="127"/>
-      <c r="T2" s="128"/>
-      <c r="U2" s="100" t="s">
+      <c r="Q2" s="136"/>
+      <c r="R2" s="136"/>
+      <c r="S2" s="136"/>
+      <c r="T2" s="137"/>
+      <c r="U2" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="V2" s="100"/>
-      <c r="W2" s="100"/>
-      <c r="X2" s="100"/>
-      <c r="Y2" s="102" t="s">
+      <c r="V2" s="108"/>
+      <c r="W2" s="108"/>
+      <c r="X2" s="108"/>
+      <c r="Y2" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="Z2" s="103"/>
-      <c r="AA2" s="103"/>
-      <c r="AB2" s="103"/>
-      <c r="AC2" s="103"/>
+      <c r="Z2" s="111"/>
+      <c r="AA2" s="111"/>
+      <c r="AB2" s="111"/>
+      <c r="AC2" s="111"/>
       <c r="AD2" s="141" t="s">
         <v>9</v>
       </c>
       <c r="AE2" s="142"/>
-      <c r="AH2" s="138"/>
-      <c r="AI2" s="138"/>
-      <c r="AJ2" s="138"/>
-      <c r="AK2" s="138"/>
-      <c r="AL2" s="138"/>
-      <c r="AM2" s="138"/>
+      <c r="AH2" s="134"/>
+      <c r="AI2" s="134"/>
+      <c r="AJ2" s="134"/>
+      <c r="AK2" s="134"/>
+      <c r="AL2" s="134"/>
+      <c r="AM2" s="134"/>
     </row>
     <row r="3" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="107"/>
-      <c r="C3" s="111"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="113"/>
-      <c r="G3" s="117"/>
-      <c r="H3" s="118"/>
-      <c r="I3" s="118"/>
-      <c r="J3" s="118"/>
-      <c r="K3" s="119"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="124"/>
-      <c r="N3" s="124"/>
-      <c r="O3" s="125"/>
-      <c r="P3" s="129"/>
-      <c r="Q3" s="130"/>
-      <c r="R3" s="130"/>
-      <c r="S3" s="130"/>
-      <c r="T3" s="131"/>
-      <c r="U3" s="101"/>
-      <c r="V3" s="101"/>
-      <c r="W3" s="101"/>
-      <c r="X3" s="101"/>
-      <c r="Y3" s="104"/>
-      <c r="Z3" s="105"/>
-      <c r="AA3" s="105"/>
-      <c r="AB3" s="105"/>
-      <c r="AC3" s="105"/>
+      <c r="B3" s="115"/>
+      <c r="C3" s="119"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="127"/>
+      <c r="L3" s="131"/>
+      <c r="M3" s="132"/>
+      <c r="N3" s="132"/>
+      <c r="O3" s="133"/>
+      <c r="P3" s="138"/>
+      <c r="Q3" s="139"/>
+      <c r="R3" s="139"/>
+      <c r="S3" s="139"/>
+      <c r="T3" s="140"/>
+      <c r="U3" s="109"/>
+      <c r="V3" s="109"/>
+      <c r="W3" s="109"/>
+      <c r="X3" s="109"/>
+      <c r="Y3" s="112"/>
+      <c r="Z3" s="113"/>
+      <c r="AA3" s="113"/>
+      <c r="AB3" s="113"/>
+      <c r="AC3" s="113"/>
       <c r="AD3" s="143"/>
       <c r="AE3" s="144"/>
-      <c r="AH3" s="138"/>
-      <c r="AI3" s="138"/>
-      <c r="AJ3" s="138"/>
-      <c r="AK3" s="138"/>
-      <c r="AL3" s="138"/>
-      <c r="AM3" s="138"/>
+      <c r="AH3" s="134"/>
+      <c r="AI3" s="134"/>
+      <c r="AJ3" s="134"/>
+      <c r="AK3" s="134"/>
+      <c r="AL3" s="134"/>
+      <c r="AM3" s="134"/>
     </row>
     <row r="4" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
@@ -1567,15 +1567,15 @@
       <c r="AC4" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="AD4" s="139">
+      <c r="AD4" s="106">
         <v>1</v>
       </c>
-      <c r="AE4" s="140" t="s">
+      <c r="AE4" s="107" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="132"/>
+      <c r="A5" s="100"/>
       <c r="B5" s="2">
         <v>1</v>
       </c>
@@ -1610,7 +1610,7 @@
       <c r="AE5" s="19"/>
     </row>
     <row r="6" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="132"/>
+      <c r="A6" s="100"/>
       <c r="B6" s="2">
         <v>2</v>
       </c>
@@ -1645,7 +1645,7 @@
       <c r="AE6" s="26"/>
     </row>
     <row r="7" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="132"/>
+      <c r="A7" s="100"/>
       <c r="B7" s="4">
         <v>3</v>
       </c>
@@ -1680,7 +1680,7 @@
       <c r="AE7" s="19"/>
     </row>
     <row r="8" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="132"/>
+      <c r="A8" s="100"/>
       <c r="B8" s="2">
         <v>4</v>
       </c>
@@ -1715,7 +1715,7 @@
       <c r="AE8" s="26"/>
     </row>
     <row r="9" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="132"/>
+      <c r="A9" s="100"/>
       <c r="B9" s="3">
         <v>5</v>
       </c>
@@ -1750,7 +1750,7 @@
       <c r="AE9" s="26"/>
     </row>
     <row r="10" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="133"/>
+      <c r="A10" s="101"/>
       <c r="B10" s="2">
         <v>6</v>
       </c>
@@ -1841,7 +1841,7 @@
       <c r="AE10" s="26"/>
     </row>
     <row r="11" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="133"/>
+      <c r="A11" s="101"/>
       <c r="B11" s="3">
         <v>7</v>
       </c>
@@ -1876,7 +1876,7 @@
       <c r="AE11" s="26"/>
     </row>
     <row r="12" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="133"/>
+      <c r="A12" s="101"/>
       <c r="B12" s="2">
         <v>8</v>
       </c>
@@ -1911,7 +1911,7 @@
       <c r="AE12" s="26"/>
     </row>
     <row r="13" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="133"/>
+      <c r="A13" s="101"/>
       <c r="B13" s="2">
         <v>9</v>
       </c>
@@ -1946,7 +1946,7 @@
       <c r="AE13" s="26"/>
     </row>
     <row r="14" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="133"/>
+      <c r="A14" s="101"/>
       <c r="B14" s="3">
         <v>10</v>
       </c>
@@ -1981,7 +1981,7 @@
       <c r="AE14" s="19"/>
     </row>
     <row r="15" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="134"/>
+      <c r="A15" s="102"/>
       <c r="B15" s="2">
         <v>11</v>
       </c>
@@ -2072,7 +2072,7 @@
       <c r="AE15" s="26"/>
     </row>
     <row r="16" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="134"/>
+      <c r="A16" s="102"/>
       <c r="B16" s="2">
         <v>12</v>
       </c>
@@ -2163,7 +2163,7 @@
       <c r="AE16" s="26"/>
     </row>
     <row r="17" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="134"/>
+      <c r="A17" s="102"/>
       <c r="B17" s="2">
         <v>13</v>
       </c>
@@ -2198,7 +2198,7 @@
       <c r="AE17" s="26"/>
     </row>
     <row r="18" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="135"/>
+      <c r="A18" s="103"/>
       <c r="B18" s="3">
         <v>14</v>
       </c>
@@ -2289,7 +2289,7 @@
       <c r="AE18" s="26"/>
     </row>
     <row r="19" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="135"/>
+      <c r="A19" s="103"/>
       <c r="B19" s="2">
         <v>15</v>
       </c>
@@ -2380,7 +2380,7 @@
       <c r="AE19" s="26"/>
     </row>
     <row r="20" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="135"/>
+      <c r="A20" s="103"/>
       <c r="B20" s="2">
         <v>16</v>
       </c>
@@ -2471,7 +2471,7 @@
       <c r="AE20" s="26"/>
     </row>
     <row r="21" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="135"/>
+      <c r="A21" s="103"/>
       <c r="B21" s="2">
         <v>17</v>
       </c>
@@ -2562,112 +2562,280 @@
       <c r="AE21" s="26"/>
     </row>
     <row r="22" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="135"/>
+      <c r="A22" s="103"/>
       <c r="B22" s="3">
         <v>18</v>
       </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="58"/>
-      <c r="M22" s="62"/>
-      <c r="N22" s="62"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="67"/>
-      <c r="Q22" s="71"/>
-      <c r="R22" s="71"/>
-      <c r="S22" s="71"/>
-      <c r="T22" s="23"/>
-      <c r="U22" s="75"/>
-      <c r="V22" s="79"/>
-      <c r="W22" s="79"/>
-      <c r="X22" s="24"/>
-      <c r="Y22" s="83"/>
-      <c r="Z22" s="87"/>
-      <c r="AA22" s="87"/>
-      <c r="AB22" s="87"/>
-      <c r="AC22" s="25"/>
-      <c r="AD22" s="91"/>
+      <c r="C22" s="35">
+        <v>5</v>
+      </c>
+      <c r="D22" s="40">
+        <v>5</v>
+      </c>
+      <c r="E22" s="45">
+        <v>5</v>
+      </c>
+      <c r="F22" s="20">
+        <v>15</v>
+      </c>
+      <c r="G22" s="50">
+        <v>5</v>
+      </c>
+      <c r="H22" s="54">
+        <v>5</v>
+      </c>
+      <c r="I22" s="54">
+        <v>5</v>
+      </c>
+      <c r="J22" s="54">
+        <v>5</v>
+      </c>
+      <c r="K22" s="21">
+        <v>20</v>
+      </c>
+      <c r="L22" s="58">
+        <v>5</v>
+      </c>
+      <c r="M22" s="62">
+        <v>5</v>
+      </c>
+      <c r="N22" s="62">
+        <v>5</v>
+      </c>
+      <c r="O22" s="22">
+        <v>15</v>
+      </c>
+      <c r="P22" s="67">
+        <v>5</v>
+      </c>
+      <c r="Q22" s="71">
+        <v>5</v>
+      </c>
+      <c r="R22" s="71">
+        <v>5</v>
+      </c>
+      <c r="S22" s="71">
+        <v>5</v>
+      </c>
+      <c r="T22" s="23">
+        <v>20</v>
+      </c>
+      <c r="U22" s="75">
+        <v>5</v>
+      </c>
+      <c r="V22" s="79">
+        <v>5</v>
+      </c>
+      <c r="W22" s="79">
+        <v>5</v>
+      </c>
+      <c r="X22" s="24">
+        <v>15</v>
+      </c>
+      <c r="Y22" s="83">
+        <v>5</v>
+      </c>
+      <c r="Z22" s="87">
+        <v>5</v>
+      </c>
+      <c r="AA22" s="87">
+        <v>5</v>
+      </c>
+      <c r="AB22" s="87">
+        <v>5</v>
+      </c>
+      <c r="AC22" s="25">
+        <v>20</v>
+      </c>
+      <c r="AD22" s="91">
+        <v>5</v>
+      </c>
       <c r="AE22" s="26"/>
     </row>
     <row r="23" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="135"/>
+      <c r="A23" s="103"/>
       <c r="B23" s="2">
         <v>19</v>
       </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="58"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="62"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="67"/>
-      <c r="Q23" s="71"/>
-      <c r="R23" s="71"/>
-      <c r="S23" s="71"/>
-      <c r="T23" s="23"/>
-      <c r="U23" s="75"/>
-      <c r="V23" s="79"/>
-      <c r="W23" s="79"/>
-      <c r="X23" s="24"/>
-      <c r="Y23" s="83"/>
-      <c r="Z23" s="87"/>
-      <c r="AA23" s="87"/>
-      <c r="AB23" s="87"/>
-      <c r="AC23" s="25"/>
-      <c r="AD23" s="91"/>
+      <c r="C23" s="35">
+        <v>5</v>
+      </c>
+      <c r="D23" s="40">
+        <v>5</v>
+      </c>
+      <c r="E23" s="45">
+        <v>5</v>
+      </c>
+      <c r="F23" s="20">
+        <v>15</v>
+      </c>
+      <c r="G23" s="50">
+        <v>5</v>
+      </c>
+      <c r="H23" s="54">
+        <v>5</v>
+      </c>
+      <c r="I23" s="54">
+        <v>5</v>
+      </c>
+      <c r="J23" s="54">
+        <v>5</v>
+      </c>
+      <c r="K23" s="21">
+        <v>20</v>
+      </c>
+      <c r="L23" s="58">
+        <v>5</v>
+      </c>
+      <c r="M23" s="62">
+        <v>5</v>
+      </c>
+      <c r="N23" s="62">
+        <v>5</v>
+      </c>
+      <c r="O23" s="22">
+        <v>15</v>
+      </c>
+      <c r="P23" s="67">
+        <v>5</v>
+      </c>
+      <c r="Q23" s="71">
+        <v>5</v>
+      </c>
+      <c r="R23" s="71">
+        <v>5</v>
+      </c>
+      <c r="S23" s="71">
+        <v>5</v>
+      </c>
+      <c r="T23" s="23">
+        <v>20</v>
+      </c>
+      <c r="U23" s="75">
+        <v>5</v>
+      </c>
+      <c r="V23" s="79">
+        <v>5</v>
+      </c>
+      <c r="W23" s="79">
+        <v>5</v>
+      </c>
+      <c r="X23" s="24">
+        <v>15</v>
+      </c>
+      <c r="Y23" s="83">
+        <v>5</v>
+      </c>
+      <c r="Z23" s="87">
+        <v>5</v>
+      </c>
+      <c r="AA23" s="87">
+        <v>5</v>
+      </c>
+      <c r="AB23" s="87">
+        <v>5</v>
+      </c>
+      <c r="AC23" s="25">
+        <v>20</v>
+      </c>
+      <c r="AD23" s="91">
+        <v>5</v>
+      </c>
       <c r="AE23" s="26"/>
     </row>
     <row r="24" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="135"/>
+      <c r="A24" s="103"/>
       <c r="B24" s="3">
         <v>20</v>
       </c>
-      <c r="C24" s="35"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="21"/>
-      <c r="L24" s="58"/>
-      <c r="M24" s="62"/>
-      <c r="N24" s="62"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="67"/>
-      <c r="Q24" s="71"/>
-      <c r="R24" s="71"/>
-      <c r="S24" s="71"/>
-      <c r="T24" s="23"/>
-      <c r="U24" s="75"/>
-      <c r="V24" s="79"/>
-      <c r="W24" s="79"/>
-      <c r="X24" s="24"/>
-      <c r="Y24" s="83"/>
-      <c r="Z24" s="87"/>
-      <c r="AA24" s="87"/>
-      <c r="AB24" s="87"/>
-      <c r="AC24" s="25"/>
-      <c r="AD24" s="91"/>
+      <c r="C24" s="35">
+        <v>5</v>
+      </c>
+      <c r="D24" s="40">
+        <v>5</v>
+      </c>
+      <c r="E24" s="45">
+        <v>5</v>
+      </c>
+      <c r="F24" s="20">
+        <v>15</v>
+      </c>
+      <c r="G24" s="50">
+        <v>4</v>
+      </c>
+      <c r="H24" s="54">
+        <v>3</v>
+      </c>
+      <c r="I24" s="54">
+        <v>4</v>
+      </c>
+      <c r="J24" s="54">
+        <v>5</v>
+      </c>
+      <c r="K24" s="21">
+        <v>16</v>
+      </c>
+      <c r="L24" s="58">
+        <v>5</v>
+      </c>
+      <c r="M24" s="62">
+        <v>4</v>
+      </c>
+      <c r="N24" s="62">
+        <v>5</v>
+      </c>
+      <c r="O24" s="22">
+        <v>14</v>
+      </c>
+      <c r="P24" s="67">
+        <v>5</v>
+      </c>
+      <c r="Q24" s="71">
+        <v>5</v>
+      </c>
+      <c r="R24" s="71">
+        <v>4</v>
+      </c>
+      <c r="S24" s="71">
+        <v>4</v>
+      </c>
+      <c r="T24" s="23">
+        <v>18</v>
+      </c>
+      <c r="U24" s="75">
+        <v>4</v>
+      </c>
+      <c r="V24" s="79">
+        <v>5</v>
+      </c>
+      <c r="W24" s="79">
+        <v>5</v>
+      </c>
+      <c r="X24" s="24">
+        <v>14</v>
+      </c>
+      <c r="Y24" s="83">
+        <v>5</v>
+      </c>
+      <c r="Z24" s="87">
+        <v>4</v>
+      </c>
+      <c r="AA24" s="87">
+        <v>4</v>
+      </c>
+      <c r="AB24" s="87">
+        <v>4</v>
+      </c>
+      <c r="AC24" s="25">
+        <v>17</v>
+      </c>
+      <c r="AD24" s="91">
+        <v>5</v>
+      </c>
       <c r="AE24" s="26"/>
     </row>
     <row r="25" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="135"/>
+      <c r="A25" s="103"/>
       <c r="B25" s="2">
         <v>21</v>
       </c>
@@ -2702,7 +2870,7 @@
       <c r="AE25" s="26"/>
     </row>
     <row r="26" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="135"/>
+      <c r="A26" s="103"/>
       <c r="B26" s="3">
         <v>22</v>
       </c>
@@ -2737,7 +2905,7 @@
       <c r="AE26" s="26"/>
     </row>
     <row r="27" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="135"/>
+      <c r="A27" s="103"/>
       <c r="B27" s="2">
         <v>23</v>
       </c>
@@ -2828,7 +2996,7 @@
       <c r="AE27" s="26"/>
     </row>
     <row r="28" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="136"/>
+      <c r="A28" s="104"/>
       <c r="B28" s="2">
         <v>24</v>
       </c>
@@ -2919,7 +3087,7 @@
       <c r="AE28" s="26"/>
     </row>
     <row r="29" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="136"/>
+      <c r="A29" s="104"/>
       <c r="B29" s="2">
         <v>25</v>
       </c>
@@ -3010,7 +3178,7 @@
       <c r="AE29" s="26"/>
     </row>
     <row r="30" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="136"/>
+      <c r="A30" s="104"/>
       <c r="B30" s="4">
         <v>26</v>
       </c>
@@ -3101,7 +3269,7 @@
       <c r="AE30" s="26"/>
     </row>
     <row r="31" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="136"/>
+      <c r="A31" s="104"/>
       <c r="B31" s="2">
         <v>27</v>
       </c>
@@ -3192,7 +3360,7 @@
       <c r="AE31" s="26"/>
     </row>
     <row r="32" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="136"/>
+      <c r="A32" s="104"/>
       <c r="B32" s="3">
         <v>28</v>
       </c>
@@ -3283,7 +3451,7 @@
       <c r="AE32" s="26"/>
     </row>
     <row r="33" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="136"/>
+      <c r="A33" s="104"/>
       <c r="B33" s="2">
         <v>29</v>
       </c>
@@ -3374,7 +3542,7 @@
       <c r="AE33" s="26"/>
     </row>
     <row r="34" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="136"/>
+      <c r="A34" s="104"/>
       <c r="B34" s="3">
         <v>30</v>
       </c>
@@ -3465,7 +3633,7 @@
       <c r="AE34" s="26"/>
     </row>
     <row r="35" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="136"/>
+      <c r="A35" s="104"/>
       <c r="B35" s="2">
         <v>31</v>
       </c>
@@ -3556,7 +3724,7 @@
       <c r="AE35" s="26"/>
     </row>
     <row r="36" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="136"/>
+      <c r="A36" s="104"/>
       <c r="B36" s="3">
         <v>32</v>
       </c>
@@ -3647,7 +3815,7 @@
       <c r="AE36" s="26"/>
     </row>
     <row r="37" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="136"/>
+      <c r="A37" s="104"/>
       <c r="B37" s="2">
         <v>33</v>
       </c>
@@ -3738,7 +3906,7 @@
       <c r="AE37" s="26"/>
     </row>
     <row r="38" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="137"/>
+      <c r="A38" s="105"/>
       <c r="B38" s="2">
         <v>34</v>
       </c>
@@ -3829,7 +3997,7 @@
       <c r="AE38" s="26"/>
     </row>
     <row r="39" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="137"/>
+      <c r="A39" s="105"/>
       <c r="B39" s="3">
         <v>35</v>
       </c>
@@ -3920,7 +4088,7 @@
       <c r="AE39" s="26"/>
     </row>
     <row r="40" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="137"/>
+      <c r="A40" s="105"/>
       <c r="B40" s="2">
         <v>36</v>
       </c>
@@ -4011,7 +4179,7 @@
       <c r="AE40" s="26"/>
     </row>
     <row r="41" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="137"/>
+      <c r="A41" s="105"/>
       <c r="B41" s="2">
         <v>37</v>
       </c>
@@ -4102,7 +4270,7 @@
       <c r="AE41" s="26"/>
     </row>
     <row r="42" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="137"/>
+      <c r="A42" s="105"/>
       <c r="B42" s="3">
         <v>38</v>
       </c>
@@ -4193,7 +4361,7 @@
       <c r="AE42" s="26"/>
     </row>
     <row r="43" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="137"/>
+      <c r="A43" s="105"/>
       <c r="B43" s="2">
         <v>39</v>
       </c>
@@ -4284,7 +4452,7 @@
       <c r="AE43" s="26"/>
     </row>
     <row r="44" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="137"/>
+      <c r="A44" s="105"/>
       <c r="B44" s="3">
         <v>40</v>
       </c>
@@ -4375,7 +4543,7 @@
       <c r="AE44" s="26"/>
     </row>
     <row r="45" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="137"/>
+      <c r="A45" s="105"/>
       <c r="B45" s="2">
         <v>41</v>
       </c>
@@ -4466,7 +4634,7 @@
       <c r="AE45" s="26"/>
     </row>
     <row r="46" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="137"/>
+      <c r="A46" s="105"/>
       <c r="B46" s="3">
         <v>42</v>
       </c>
@@ -4557,7 +4725,7 @@
       <c r="AE46" s="26"/>
     </row>
     <row r="47" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="137"/>
+      <c r="A47" s="105"/>
       <c r="B47" s="2">
         <v>43</v>
       </c>
@@ -4648,7 +4816,7 @@
       <c r="AE47" s="26"/>
     </row>
     <row r="48" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="137"/>
+      <c r="A48" s="105"/>
       <c r="B48" s="3">
         <v>44</v>
       </c>
@@ -4739,7 +4907,7 @@
       <c r="AE48" s="26"/>
     </row>
     <row r="49" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="137"/>
+      <c r="A49" s="105"/>
       <c r="B49" s="4">
         <v>45</v>
       </c>
@@ -4866,15 +5034,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="AH2:AM3"/>
+    <mergeCell ref="P2:T3"/>
+    <mergeCell ref="AD2:AE3"/>
     <mergeCell ref="U2:X3"/>
     <mergeCell ref="Y2:AC3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:F3"/>
     <mergeCell ref="G2:K3"/>
     <mergeCell ref="L2:O3"/>
-    <mergeCell ref="AH2:AM3"/>
-    <mergeCell ref="P2:T3"/>
-    <mergeCell ref="AD2:AE3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>